<commit_message>
meilleure detection si nom feuille/colonne est conforme
</commit_message>
<xml_diff>
--- a/Inventaireproduitschimiques.xlsx
+++ b/Inventaireproduitschimiques.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Produits_chimiques" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,22 +20,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="569">
   <si>
-    <t>Nom francais|type='string'</t>
-  </si>
-  <si>
-    <t>Nom anglais|type='string'</t>
+    <t>Nom_francais|type='string'</t>
+  </si>
+  <si>
+    <t>Nom_anglais|type='string'</t>
   </si>
   <si>
     <t>Synonyme|type='string'</t>
   </si>
   <si>
-    <t>N CAS|type='string'</t>
+    <t>NCAS|type='string'</t>
   </si>
   <si>
     <t>Formule|type='string'</t>
   </si>
   <si>
-    <t>Masse molaire gmol|type='float'</t>
+    <t>Masse_molaire_gmol|type='float'</t>
   </si>
   <si>
     <t>Forme|type='string'</t>
@@ -44,28 +44,28 @@
     <t>Symbole|type='string'</t>
   </si>
   <si>
-    <t>Mentions de danger|reference=Mentions_de_danger</t>
-  </si>
-  <si>
-    <t>Conseils de prudence|reference=Conseils_de_prudence</t>
-  </si>
-  <si>
-    <t>FDS (piece jointe)</t>
-  </si>
-  <si>
-    <t>Hazard statements</t>
-  </si>
-  <si>
-    <t>Precautionary statements</t>
-  </si>
-  <si>
-    <t>MSDS (piece jointe)</t>
-  </si>
-  <si>
-    <t>Lien FDS</t>
-  </si>
-  <si>
-    <t>Lien MSDS</t>
+    <t>Mentions_de_danger|reference=Mentions_de_danger</t>
+  </si>
+  <si>
+    <t>Conseils_de_prudence|reference=Conseils_de_prudence</t>
+  </si>
+  <si>
+    <t>FDS_piece_jointe</t>
+  </si>
+  <si>
+    <t>Hazard_statements</t>
+  </si>
+  <si>
+    <t>Precautionary_statements</t>
+  </si>
+  <si>
+    <t>MSDS_piece_jointe</t>
+  </si>
+  <si>
+    <t>Lien_FDS</t>
+  </si>
+  <si>
+    <t>Lien_MSDS</t>
   </si>
   <si>
     <t>(+)-Bicuculline</t>
@@ -1557,7 +1557,7 @@
     <t>Codes|idthis</t>
   </si>
   <si>
-    <t>Mentions de danger|type='string'</t>
+    <t>Mentions_de_danger|type='string'</t>
   </si>
   <si>
     <t>Explosif instable</t>
@@ -2088,10 +2088,10 @@
     <t>To avoid risks to human health and the environment, comply with the instructions for use</t>
   </si>
   <si>
-    <t>Conseils de prudence|type='string'</t>
-  </si>
-  <si>
-    <t>Precautionary statements|type='string'</t>
+    <t>Conseils_de_prudence|type='string'</t>
+  </si>
+  <si>
+    <t>Precautionary_statements|type='string'</t>
   </si>
   <si>
     <t>En cas de consultation d’un médecin, garder à disposition le récipient ou l’étiquette</t>
@@ -2730,16 +2730,16 @@
     <t>ColonneT</t>
   </si>
   <si>
-    <t>Produits chimiques</t>
-  </si>
-  <si>
-    <t>Nom francais</t>
-  </si>
-  <si>
-    <t>Nom anglais</t>
-  </si>
-  <si>
-    <t>Mentions de danger</t>
+    <t>Produits_chimiques</t>
+  </si>
+  <si>
+    <t>Nom_francais</t>
+  </si>
+  <si>
+    <t>Nom_anglais</t>
+  </si>
+  <si>
+    <t>Mentions_de_danger</t>
   </si>
 </sst>
 </file>
@@ -2880,8 +2880,8 @@
   </sheetPr>
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A20" activeCellId="0" pane="topLeft" sqref="20:37"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="M1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -3685,8 +3685,8 @@
   </sheetPr>
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="1" pane="topLeft" sqref="20:37 B1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -4692,8 +4692,8 @@
   </sheetPr>
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B8" activeCellId="1" pane="topLeft" sqref="20:37 B8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -4703,7 +4703,7 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.85490196078431"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="1">
       <c r="A1" s="4" t="s">
         <v>173</v>
       </c>
@@ -5885,14 +5885,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="20:37 A4"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.46666666666667"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>562</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>564</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>565</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>567</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>565</v>
       </c>

</xml_diff>

<commit_message>
multiples fichiers avec reference corrigé
</commit_message>
<xml_diff>
--- a/Inventaireproduitschimiques.xlsx
+++ b/Inventaireproduitschimiques.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Produits_chimiques" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="570">
   <si>
     <t>Nom_francais|type='string'</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Masse_molaire_gmol|type='float'</t>
+  </si>
+  <si>
+    <t>Masse_molaire_gmoli|type='float'</t>
   </si>
   <si>
     <t>Forme|type='string'</t>
@@ -2749,7 +2752,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -2793,12 +2796,6 @@
       <charset val="1"/>
       <family val="2"/>
       <i val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <color rgb="00000000"/>
       <sz val="11"/>
     </font>
@@ -2852,15 +2849,14 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -2878,29 +2874,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="M1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G2" activeCellId="0" pane="topLeft" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.7137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8274509803922"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2352941176471"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.7372549019608"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="44.1803921568627"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.8392156862745"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.1725490196078"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.7254901960784"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.0666666666667"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1372549019608"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.3529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8862745098039"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="18.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3058823529412"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8509803921569"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="44.3647058823529"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.9333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.2901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.8745098039216"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="33.2"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.2196078431373"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.4235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="1" s="1">
@@ -2952,25 +2948,28 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>367.35</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>19</v>
+      <c r="G2" s="0" t="n">
+        <v>467.35</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>20</v>
@@ -2982,10 +2981,10 @@
         <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>24</v>
@@ -2999,34 +2998,37 @@
       <c r="P2" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="Q2" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>186.17</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>32</v>
+      <c r="G3" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>33</v>
@@ -3034,57 +3036,63 @@
       <c r="P3" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="Q3" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="4">
       <c r="B4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>129.16</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>39</v>
+      <c r="G4" s="0" t="n">
+        <v>510</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>430.71</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>44</v>
+      <c r="G5" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>45</v>
@@ -3092,28 +3100,31 @@
       <c r="P5" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="Q5" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>213.66</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>19</v>
+      <c r="G6" s="0" t="n">
+        <v>665</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>52</v>
@@ -3121,7 +3132,7 @@
       <c r="J6" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="K6" s="0" t="s">
         <v>54</v>
       </c>
       <c r="M6" s="0" t="s">
@@ -3130,51 +3141,57 @@
       <c r="N6" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="O6" s="0" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="7">
       <c r="B7" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>325.06</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>61</v>
+      <c r="G7" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>412.44</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>19</v>
+      <c r="G8" s="0" t="n">
+        <v>544</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>67</v>
@@ -3183,10 +3200,10 @@
         <v>68</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="M8" s="0" t="s">
         <v>70</v>
@@ -3200,40 +3217,43 @@
       <c r="P8" s="0" t="s">
         <v>73</v>
       </c>
+      <c r="Q8" s="0" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>108.14</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>19</v>
+      <c r="G9" s="0" t="n">
+        <v>498</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>79</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M9" s="0" t="s">
         <v>81</v>
@@ -3247,43 +3267,46 @@
       <c r="P9" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="Q9" s="0" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>122.19</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>19</v>
+      <c r="G10" s="0" t="n">
+        <v>150</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>85</v>
+      <c r="K10" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>93</v>
@@ -3297,46 +3320,49 @@
       <c r="P10" s="0" t="s">
         <v>96</v>
       </c>
+      <c r="Q10" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>335.32</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>19</v>
+      <c r="G11" s="0" t="n">
+        <v>648</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>67</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>101</v>
+      <c r="K11" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="M11" s="0" t="s">
         <v>70</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>103</v>
@@ -3344,31 +3370,34 @@
       <c r="P11" s="0" t="s">
         <v>104</v>
       </c>
+      <c r="Q11" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>301.69</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>109</v>
+      <c r="G12" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="O12" s="0" t="s">
         <v>110</v>
@@ -3376,42 +3405,45 @@
       <c r="P12" s="0" t="s">
         <v>111</v>
       </c>
+      <c r="Q12" s="0" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>164.18</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>19</v>
+      <c r="G13" s="0" t="n">
+        <v>224</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>67</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="N13" s="0" t="s">
+      <c r="K13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="0" t="s">
         <v>118</v>
       </c>
       <c r="O13" s="0" t="s">
@@ -3420,28 +3452,31 @@
       <c r="P13" s="0" t="s">
         <v>120</v>
       </c>
+      <c r="Q13" s="0" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>214.27</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>19</v>
+      <c r="G14" s="0" t="n">
+        <v>214.27</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>126</v>
@@ -3450,10 +3485,10 @@
         <v>127</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="N14" s="0" t="s">
         <v>128</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="O14" s="0" t="s">
         <v>129</v>
@@ -3461,39 +3496,42 @@
       <c r="P14" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="Q14" s="0" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>881.7</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>19</v>
+      <c r="G15" s="0" t="n">
+        <v>881.7</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="N15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>136</v>
       </c>
       <c r="O15" s="0" t="s">
@@ -3502,40 +3540,43 @@
       <c r="P15" s="0" t="s">
         <v>138</v>
       </c>
+      <c r="Q15" s="0" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>94.11</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>19</v>
+      <c r="G16" s="0" t="n">
+        <v>94.11</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>144</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="N16" s="0" t="s">
         <v>145</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>140</v>
       </c>
       <c r="O16" s="0" t="s">
         <v>146</v>
@@ -3543,40 +3584,43 @@
       <c r="P16" s="0" t="s">
         <v>147</v>
       </c>
+      <c r="Q16" s="0" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>201.06</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>19</v>
+      <c r="G17" s="0" t="n">
+        <v>201.06</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="N17" s="0" t="s">
-        <v>152</v>
+        <v>69</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>149</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>153</v>
@@ -3584,28 +3628,31 @@
       <c r="P17" s="0" t="s">
         <v>154</v>
       </c>
+      <c r="Q17" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>387.51</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>19</v>
+      <c r="G18" s="0" t="n">
+        <v>387.51</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>160</v>
@@ -3614,10 +3661,10 @@
         <v>161</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="N18" s="0" t="s">
         <v>162</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>156</v>
       </c>
       <c r="O18" s="0" t="s">
         <v>163</v>
@@ -3625,46 +3672,52 @@
       <c r="P18" s="0" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
+      <c r="Q18" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>246.19</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>19</v>
+      <c r="G19" s="0" t="n">
+        <v>246.19</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="N19" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="O19" s="0" t="s">
         <v>171</v>
       </c>
       <c r="P19" s="0" t="s">
         <v>172</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3685,25 +3738,25 @@
   </sheetPr>
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.85490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="170.21568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="170.917647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
+      <c r="A1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
+      <c r="B1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -3711,10 +3764,10 @@
         <v>200</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C2" s="5" t="s">
         <v>176</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
@@ -3722,10 +3775,10 @@
         <v>201</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>178</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
@@ -3733,10 +3786,10 @@
         <v>202</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="C4" s="5" t="s">
         <v>180</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
@@ -3744,10 +3797,10 @@
         <v>203</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="5" t="s">
         <v>182</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="6">
@@ -3755,10 +3808,10 @@
         <v>204</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="5" t="s">
         <v>184</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
@@ -3766,10 +3819,10 @@
         <v>205</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C7" s="5" t="s">
         <v>186</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
@@ -3777,10 +3830,10 @@
         <v>220</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8" s="5" t="s">
         <v>188</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
@@ -3788,10 +3841,10 @@
         <v>221</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="C9" s="5" t="s">
         <v>190</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>191</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
@@ -3799,10 +3852,10 @@
         <v>222</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>192</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
@@ -3810,10 +3863,10 @@
         <v>223</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C11" s="5" t="s">
         <v>194</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
@@ -3821,10 +3874,10 @@
         <v>224</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="5" t="s">
         <v>196</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
@@ -3832,10 +3885,10 @@
         <v>225</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>198</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
@@ -3843,10 +3896,10 @@
         <v>226</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="C14" s="5" t="s">
         <v>200</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="15">
@@ -3854,10 +3907,10 @@
         <v>228</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>202</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>203</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
@@ -3865,10 +3918,10 @@
         <v>240</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" s="5" t="s">
         <v>204</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
@@ -3876,10 +3929,10 @@
         <v>241</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="C17" s="5" t="s">
         <v>206</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
@@ -3887,10 +3940,10 @@
         <v>242</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="5" t="s">
         <v>208</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>209</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="19">
@@ -3898,10 +3951,10 @@
         <v>250</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C19" s="5" t="s">
         <v>210</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20">
@@ -3909,10 +3962,10 @@
         <v>251</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C20" s="5" t="s">
         <v>212</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="21">
@@ -3920,10 +3973,10 @@
         <v>252</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="5" t="s">
         <v>214</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="22">
@@ -3931,10 +3984,10 @@
         <v>260</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="C22" s="5" t="s">
         <v>216</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>217</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
@@ -3942,10 +3995,10 @@
         <v>261</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="C23" s="5" t="s">
         <v>218</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="24">
@@ -3953,10 +4006,10 @@
         <v>270</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="C24" s="5" t="s">
         <v>220</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="25">
@@ -3964,10 +4017,10 @@
         <v>271</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="C25" s="5" t="s">
         <v>222</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>223</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
@@ -3975,10 +4028,10 @@
         <v>272</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="C26" s="5" t="s">
         <v>224</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="27">
@@ -3986,10 +4039,10 @@
         <v>280</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C27" s="5" t="s">
         <v>226</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="28">
@@ -3997,10 +4050,10 @@
         <v>281</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="C28" s="5" t="s">
         <v>228</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="29">
@@ -4008,10 +4061,10 @@
         <v>290</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C29" s="5" t="s">
         <v>230</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
@@ -4019,10 +4072,10 @@
         <v>300</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="C30" s="5" t="s">
         <v>232</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="31">
@@ -4030,10 +4083,10 @@
         <v>301</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C31" s="5" t="s">
         <v>234</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="32">
@@ -4041,10 +4094,10 @@
         <v>302</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="C32" s="5" t="s">
         <v>236</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="33">
@@ -4052,10 +4105,10 @@
         <v>304</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="C33" s="5" t="s">
         <v>238</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="34">
@@ -4063,10 +4116,10 @@
         <v>310</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="C34" s="5" t="s">
         <v>240</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="35">
@@ -4074,10 +4127,10 @@
         <v>311</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="C35" s="5" t="s">
         <v>242</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="36">
@@ -4085,10 +4138,10 @@
         <v>312</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="C36" s="5" t="s">
         <v>244</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="37">
@@ -4096,10 +4149,10 @@
         <v>314</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="C37" s="5" t="s">
         <v>246</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="38">
@@ -4107,10 +4160,10 @@
         <v>315</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="C38" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="39">
@@ -4118,10 +4171,10 @@
         <v>317</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="C39" s="5" t="s">
         <v>250</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="40">
@@ -4129,10 +4182,10 @@
         <v>318</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="C40" s="5" t="s">
         <v>252</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="41">
@@ -4140,10 +4193,10 @@
         <v>319</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="C41" s="5" t="s">
         <v>254</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="42">
@@ -4151,10 +4204,10 @@
         <v>330</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="C42" s="5" t="s">
         <v>256</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>257</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="43">
@@ -4162,10 +4215,10 @@
         <v>331</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="C43" s="5" t="s">
         <v>258</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>259</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="44">
@@ -4173,10 +4226,10 @@
         <v>332</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="C44" s="5" t="s">
         <v>260</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>261</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="45">
@@ -4184,10 +4237,10 @@
         <v>334</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="C45" s="5" t="s">
         <v>262</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="46">
@@ -4195,10 +4248,10 @@
         <v>335</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="C46" s="5" t="s">
         <v>264</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="47">
@@ -4206,10 +4259,10 @@
         <v>336</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="C47" s="5" t="s">
         <v>266</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="48">
@@ -4217,10 +4270,10 @@
         <v>340</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C48" s="5" t="s">
         <v>268</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="49">
@@ -4228,10 +4281,10 @@
         <v>341</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="C49" s="5" t="s">
         <v>270</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="50">
@@ -4239,10 +4292,10 @@
         <v>350</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="C50" s="5" t="s">
         <v>272</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="51">
@@ -4250,10 +4303,10 @@
         <v>351</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="C51" s="5" t="s">
         <v>274</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>275</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="52">
@@ -4261,10 +4314,10 @@
         <v>360</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="C52" s="5" t="s">
         <v>276</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>277</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="53">
@@ -4272,10 +4325,10 @@
         <v>361</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="C53" s="5" t="s">
         <v>278</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="54">
@@ -4283,10 +4336,10 @@
         <v>362</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="C54" s="5" t="s">
         <v>280</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>281</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="55">
@@ -4294,10 +4347,10 @@
         <v>370</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="C55" s="5" t="s">
         <v>282</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>283</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="56">
@@ -4305,10 +4358,10 @@
         <v>371</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="C56" s="5" t="s">
         <v>284</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>285</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="57">
@@ -4316,10 +4369,10 @@
         <v>372</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="C57" s="5" t="s">
         <v>286</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>287</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="58">
@@ -4327,10 +4380,10 @@
         <v>373</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="C58" s="5" t="s">
         <v>288</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>289</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="59">
@@ -4338,10 +4391,10 @@
         <v>400</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="C59" s="5" t="s">
         <v>290</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>291</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="60">
@@ -4349,10 +4402,10 @@
         <v>410</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="C60" s="5" t="s">
         <v>292</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>293</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="61">
@@ -4360,10 +4413,10 @@
         <v>411</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="C61" s="5" t="s">
         <v>294</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>295</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="62">
@@ -4371,10 +4424,10 @@
         <v>412</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="C62" s="5" t="s">
         <v>296</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>297</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="63">
@@ -4382,10 +4435,10 @@
         <v>413</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="C63" s="5" t="s">
         <v>298</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>299</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="64">
@@ -4393,10 +4446,10 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="C64" s="5" t="s">
         <v>300</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>301</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="65">
@@ -4404,10 +4457,10 @@
         <v>6</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="C65" s="5" t="s">
         <v>302</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>303</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="66">
@@ -4415,10 +4468,10 @@
         <v>14</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="C66" s="5" t="s">
         <v>304</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>305</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="67">
@@ -4426,10 +4479,10 @@
         <v>18</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="C67" s="5" t="s">
         <v>306</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>307</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="68">
@@ -4437,10 +4490,10 @@
         <v>19</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="C68" s="5" t="s">
         <v>308</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>309</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="69">
@@ -4448,10 +4501,10 @@
         <v>44</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="C69" s="5" t="s">
         <v>310</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>311</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="70">
@@ -4459,10 +4512,10 @@
         <v>29</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="C70" s="5" t="s">
         <v>312</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>313</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="71">
@@ -4470,10 +4523,10 @@
         <v>31</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="C71" s="5" t="s">
         <v>314</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="72">
@@ -4481,10 +4534,10 @@
         <v>32</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="C72" s="5" t="s">
         <v>316</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>317</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="73">
@@ -4492,10 +4545,10 @@
         <v>66</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="C73" s="5" t="s">
         <v>318</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>319</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="74">
@@ -4503,10 +4556,10 @@
         <v>70</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="C74" s="5" t="s">
         <v>320</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>321</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="75">
@@ -4514,10 +4567,10 @@
         <v>71</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="C75" s="5" t="s">
         <v>322</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="76">
@@ -4525,10 +4578,10 @@
         <v>59</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="C76" s="5" t="s">
         <v>324</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>325</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="77">
@@ -4536,10 +4589,10 @@
         <v>2010</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C77" s="5" t="s">
         <v>326</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>327</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="78">
@@ -4547,10 +4600,10 @@
         <v>2011</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="C78" s="5" t="s">
         <v>328</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>329</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="79">
@@ -4558,10 +4611,10 @@
         <v>2020</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="C79" s="5" t="s">
         <v>330</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>331</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="80">
@@ -4569,10 +4622,10 @@
         <v>2030</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="C80" s="5" t="s">
         <v>332</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="81">
@@ -4580,10 +4633,10 @@
         <v>2040</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="C81" s="5" t="s">
         <v>334</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="82">
@@ -4591,10 +4644,10 @@
         <v>2050</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="C82" s="5" t="s">
         <v>336</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="83">
@@ -4602,10 +4655,10 @@
         <v>2060</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="C83" s="5" t="s">
         <v>338</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>339</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="84">
@@ -4613,10 +4666,10 @@
         <v>2070</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C84" s="5" t="s">
         <v>340</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>341</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="85">
@@ -4624,10 +4677,10 @@
         <v>2080</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="C85" s="5" t="s">
         <v>342</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>343</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="86">
@@ -4635,10 +4688,10 @@
         <v>2090</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="C86" s="5" t="s">
         <v>344</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>345</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="87">
@@ -4646,10 +4699,10 @@
         <v>2091</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C87" s="5" t="s">
         <v>346</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>347</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="88">
@@ -4657,10 +4710,10 @@
         <v>2100</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="C88" s="5" t="s">
         <v>348</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>349</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="89">
@@ -4668,10 +4721,10 @@
         <v>4100</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="C89" s="5" t="s">
         <v>350</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -4697,21 +4750,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8274509803922"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="140.886274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="159.392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="141.474509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="160.054901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
+      <c r="A1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>352</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>353</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -4719,10 +4772,10 @@
         <v>101</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="C2" s="5" t="s">
         <v>354</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>355</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
@@ -4730,10 +4783,10 @@
         <v>102</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>356</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>357</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
@@ -4741,10 +4794,10 @@
         <v>103</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="C4" s="5" t="s">
         <v>358</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>359</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
@@ -4752,10 +4805,10 @@
         <v>200</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="C5" s="5" t="s">
         <v>360</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>361</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="6">
@@ -4763,10 +4816,10 @@
         <v>201</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>361</v>
-      </c>
-      <c r="C6" s="5" t="s">
         <v>362</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>363</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
@@ -4774,10 +4827,10 @@
         <v>210</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="C7" s="5" t="s">
         <v>364</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
@@ -4785,10 +4838,10 @@
         <v>211</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>365</v>
-      </c>
-      <c r="C8" s="5" t="s">
         <v>366</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
@@ -4796,10 +4849,10 @@
         <v>220</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="C9" s="5" t="s">
         <v>368</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>369</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
@@ -4807,10 +4860,10 @@
         <v>221</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>370</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
@@ -4818,10 +4871,10 @@
         <v>222</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="C11" s="5" t="s">
         <v>372</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
@@ -4829,10 +4882,10 @@
         <v>223</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="C12" s="5" t="s">
         <v>374</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
@@ -4840,10 +4893,10 @@
         <v>230</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>376</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>377</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
@@ -4851,10 +4904,10 @@
         <v>231</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="C14" s="5" t="s">
         <v>378</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>379</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="15">
@@ -4862,10 +4915,10 @@
         <v>232</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>380</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>381</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
@@ -4873,10 +4926,10 @@
         <v>233</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="C16" s="5" t="s">
         <v>382</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
@@ -4884,10 +4937,10 @@
         <v>234</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="C17" s="5" t="s">
         <v>384</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>385</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
@@ -4895,10 +4948,10 @@
         <v>235</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="C18" s="5" t="s">
         <v>386</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>387</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="19">
@@ -4906,10 +4959,10 @@
         <v>240</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="C19" s="5" t="s">
         <v>388</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>389</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20">
@@ -4917,10 +4970,10 @@
         <v>241</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="C20" s="5" t="s">
         <v>390</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>391</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="21">
@@ -4928,10 +4981,10 @@
         <v>242</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="C21" s="5" t="s">
         <v>392</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="22">
@@ -4939,10 +4992,10 @@
         <v>243</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="C22" s="5" t="s">
         <v>394</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>395</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
@@ -4950,10 +5003,10 @@
         <v>244</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="C23" s="5" t="s">
         <v>396</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="24">
@@ -4961,10 +5014,10 @@
         <v>250</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="C24" s="5" t="s">
         <v>398</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>399</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="25">
@@ -4972,10 +5025,10 @@
         <v>251</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="C25" s="5" t="s">
         <v>400</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
@@ -4983,10 +5036,10 @@
         <v>260</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="C26" s="5" t="s">
         <v>402</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="27">
@@ -4994,10 +5047,10 @@
         <v>261</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="C27" s="5" t="s">
         <v>404</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="28">
@@ -5005,10 +5058,10 @@
         <v>262</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="C28" s="5" t="s">
         <v>406</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="29">
@@ -5016,10 +5069,10 @@
         <v>263</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C29" s="5" t="s">
         <v>408</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>409</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
@@ -5027,10 +5080,10 @@
         <v>264</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="C30" s="5" t="s">
         <v>410</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>411</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="31">
@@ -5038,10 +5091,10 @@
         <v>270</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="C31" s="5" t="s">
         <v>412</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="32">
@@ -5049,10 +5102,10 @@
         <v>271</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="C32" s="5" t="s">
         <v>414</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="33">
@@ -5060,10 +5113,10 @@
         <v>272</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="C33" s="5" t="s">
         <v>416</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>417</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="34">
@@ -5071,10 +5124,10 @@
         <v>273</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="C34" s="5" t="s">
         <v>418</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>419</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="35">
@@ -5082,10 +5135,10 @@
         <v>280</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="C35" s="5" t="s">
         <v>420</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="36">
@@ -5093,10 +5146,10 @@
         <v>281</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="C36" s="5" t="s">
         <v>422</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="37">
@@ -5104,10 +5157,10 @@
         <v>282</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>423</v>
-      </c>
-      <c r="C37" s="5" t="s">
         <v>424</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="38">
@@ -5115,10 +5168,10 @@
         <v>283</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="C38" s="5" t="s">
         <v>426</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="39">
@@ -5126,10 +5179,10 @@
         <v>284</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="C39" s="5" t="s">
         <v>428</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="40">
@@ -5137,10 +5190,10 @@
         <v>285</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>429</v>
-      </c>
-      <c r="C40" s="5" t="s">
         <v>430</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="41">
@@ -5148,10 +5201,10 @@
         <v>301</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="C41" s="5" t="s">
         <v>432</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="42">
@@ -5159,10 +5212,10 @@
         <v>302</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="C42" s="5" t="s">
         <v>434</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="43">
@@ -5170,10 +5223,10 @@
         <v>303</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="C43" s="5" t="s">
         <v>436</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="44">
@@ -5181,10 +5234,10 @@
         <v>304</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="C44" s="5" t="s">
         <v>438</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="45">
@@ -5192,10 +5245,10 @@
         <v>305</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="C45" s="5" t="s">
         <v>440</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="46">
@@ -5203,10 +5256,10 @@
         <v>306</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="C46" s="5" t="s">
         <v>442</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="47">
@@ -5214,10 +5267,10 @@
         <v>307</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>443</v>
-      </c>
-      <c r="C47" s="5" t="s">
         <v>444</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="48">
@@ -5225,10 +5278,10 @@
         <v>308</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="C48" s="5" t="s">
         <v>446</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="49">
@@ -5236,10 +5289,10 @@
         <v>309</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>447</v>
-      </c>
-      <c r="C49" s="5" t="s">
         <v>448</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>449</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="50">
@@ -5247,10 +5300,10 @@
         <v>310</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="C50" s="5" t="s">
         <v>450</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>451</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="51">
@@ -5258,10 +5311,10 @@
         <v>311</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>451</v>
-      </c>
-      <c r="C51" s="5" t="s">
         <v>452</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>453</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="52">
@@ -5269,10 +5322,10 @@
         <v>312</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="C52" s="5" t="s">
         <v>454</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="53">
@@ -5280,10 +5333,10 @@
         <v>313</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="C53" s="5" t="s">
         <v>456</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>457</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="54">
@@ -5291,10 +5344,10 @@
         <v>314</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="C54" s="5" t="s">
         <v>458</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>459</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="55">
@@ -5302,10 +5355,10 @@
         <v>315</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="C55" s="5" t="s">
         <v>460</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>461</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="56">
@@ -5313,10 +5366,10 @@
         <v>320</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>461</v>
-      </c>
-      <c r="C56" s="5" t="s">
         <v>462</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>463</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="57">
@@ -5324,10 +5377,10 @@
         <v>321</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="C57" s="5" t="s">
         <v>464</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="58">
@@ -5335,10 +5388,10 @@
         <v>322</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>465</v>
-      </c>
-      <c r="C58" s="5" t="s">
         <v>466</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>467</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="59">
@@ -5346,10 +5399,10 @@
         <v>330</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="C59" s="5" t="s">
         <v>468</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>469</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="60">
@@ -5357,10 +5410,10 @@
         <v>331</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="C60" s="5" t="s">
         <v>470</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>471</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="61">
@@ -5368,10 +5421,10 @@
         <v>332</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="C61" s="5" t="s">
         <v>472</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>473</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="62">
@@ -5379,10 +5432,10 @@
         <v>333</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="C62" s="5" t="s">
         <v>474</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="63">
@@ -5390,10 +5443,10 @@
         <v>334</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="C63" s="5" t="s">
         <v>476</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>477</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="64">
@@ -5401,10 +5454,10 @@
         <v>335</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>477</v>
-      </c>
-      <c r="C64" s="5" t="s">
         <v>478</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>479</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="65">
@@ -5412,10 +5465,10 @@
         <v>336</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="C65" s="5" t="s">
         <v>480</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>481</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="66">
@@ -5423,10 +5476,10 @@
         <v>337</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C66" s="5" t="s">
         <v>482</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>483</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="67">
@@ -5434,10 +5487,10 @@
         <v>338</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="C67" s="5" t="s">
         <v>484</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>485</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="68">
@@ -5445,10 +5498,10 @@
         <v>340</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="C68" s="5" t="s">
         <v>486</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>487</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="69">
@@ -5456,10 +5509,10 @@
         <v>341</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="C69" s="5" t="s">
         <v>488</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>489</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="70">
@@ -5467,10 +5520,10 @@
         <v>342</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="C70" s="5" t="s">
         <v>490</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>491</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="71">
@@ -5478,10 +5531,10 @@
         <v>350</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="C71" s="5" t="s">
         <v>492</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>493</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="72">
@@ -5489,10 +5542,10 @@
         <v>351</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="C72" s="5" t="s">
         <v>494</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="73">
@@ -5500,10 +5553,10 @@
         <v>352</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="C73" s="5" t="s">
         <v>496</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>497</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="74">
@@ -5511,10 +5564,10 @@
         <v>353</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>497</v>
-      </c>
-      <c r="C74" s="5" t="s">
         <v>498</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>499</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="75">
@@ -5522,10 +5575,10 @@
         <v>360</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="C75" s="5" t="s">
         <v>500</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>501</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="76">
@@ -5533,10 +5586,10 @@
         <v>361</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="C76" s="5" t="s">
         <v>502</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="77">
@@ -5544,10 +5597,10 @@
         <v>362</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="C77" s="5" t="s">
         <v>504</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="78">
@@ -5555,10 +5608,10 @@
         <v>363</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>505</v>
-      </c>
-      <c r="C78" s="5" t="s">
         <v>506</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="79">
@@ -5566,10 +5619,10 @@
         <v>370</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>507</v>
-      </c>
-      <c r="C79" s="5" t="s">
         <v>508</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>509</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="80">
@@ -5577,10 +5630,10 @@
         <v>371</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="C80" s="5" t="s">
         <v>510</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>511</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="81">
@@ -5588,10 +5641,10 @@
         <v>372</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="C81" s="5" t="s">
         <v>512</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>513</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="82">
@@ -5599,10 +5652,10 @@
         <v>373</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="C82" s="5" t="s">
         <v>514</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="83">
@@ -5610,10 +5663,10 @@
         <v>374</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="C83" s="5" t="s">
         <v>516</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="84">
@@ -5621,10 +5674,10 @@
         <v>375</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="C84" s="5" t="s">
         <v>518</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>519</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="85">
@@ -5632,10 +5685,10 @@
         <v>376</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="C85" s="5" t="s">
         <v>520</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>521</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="86">
@@ -5643,10 +5696,10 @@
         <v>377</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="C86" s="5" t="s">
         <v>522</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>523</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="87">
@@ -5654,10 +5707,10 @@
         <v>378</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="C87" s="5" t="s">
         <v>524</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>525</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="88">
@@ -5665,10 +5718,10 @@
         <v>380</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="C88" s="5" t="s">
         <v>526</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>527</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="89">
@@ -5676,10 +5729,10 @@
         <v>381</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>527</v>
-      </c>
-      <c r="C89" s="5" t="s">
         <v>528</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>529</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="90">
@@ -5687,10 +5740,10 @@
         <v>390</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="C90" s="5" t="s">
         <v>530</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>531</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="91">
@@ -5698,10 +5751,10 @@
         <v>391</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="C91" s="5" t="s">
         <v>532</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>533</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="92">
@@ -5709,10 +5762,10 @@
         <v>401</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>533</v>
-      </c>
-      <c r="C92" s="5" t="s">
         <v>534</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>535</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="93">
@@ -5720,10 +5773,10 @@
         <v>402</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="C93" s="5" t="s">
         <v>536</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>537</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="94">
@@ -5731,10 +5784,10 @@
         <v>403</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>537</v>
-      </c>
-      <c r="C94" s="5" t="s">
         <v>538</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>539</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="95">
@@ -5742,10 +5795,10 @@
         <v>404</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C95" s="5" t="s">
         <v>540</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>541</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="96">
@@ -5753,10 +5806,10 @@
         <v>405</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="C96" s="5" t="s">
         <v>542</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>543</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="97">
@@ -5764,10 +5817,10 @@
         <v>406</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="C97" s="5" t="s">
         <v>544</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>545</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="98">
@@ -5775,10 +5828,10 @@
         <v>407</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="C98" s="5" t="s">
         <v>546</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>547</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="99">
@@ -5786,10 +5839,10 @@
         <v>410</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>547</v>
-      </c>
-      <c r="C99" s="5" t="s">
         <v>548</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>549</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="100">
@@ -5797,10 +5850,10 @@
         <v>411</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>549</v>
-      </c>
-      <c r="C100" s="5" t="s">
         <v>550</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>551</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="101">
@@ -5808,10 +5861,10 @@
         <v>412</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>551</v>
-      </c>
-      <c r="C101" s="5" t="s">
         <v>552</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>553</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="102">
@@ -5819,10 +5872,10 @@
         <v>413</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="C102" s="5" t="s">
         <v>554</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>555</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="103">
@@ -5830,10 +5883,10 @@
         <v>420</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>555</v>
-      </c>
-      <c r="C103" s="5" t="s">
         <v>556</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>557</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="104">
@@ -5841,10 +5894,10 @@
         <v>422</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>557</v>
-      </c>
-      <c r="C104" s="5" t="s">
         <v>558</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>559</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="105">
@@ -5852,18 +5905,18 @@
         <v>501</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>559</v>
-      </c>
-      <c r="C105" s="5" t="s">
         <v>560</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>561</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="106">
       <c r="A106" s="0" t="n">
         <v>502</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>561</v>
+      <c r="B106" s="4" t="s">
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -5889,51 +5942,51 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.46666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.50196078431373"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+        <v>565</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>567</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>565</v>
-      </c>
       <c r="B3" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>